<commit_message>
adding additional outfiles from example test
</commit_message>
<xml_diff>
--- a/examples/GM16736_vs_HG002/GM16736_vs_HG002.xlsx
+++ b/examples/GM16736_vs_HG002/GM16736_vs_HG002.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="SV_calls" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="CNV_and_Aneuploidy_calls" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="CNV_metrics" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SV_calls" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CNV_and_Aneuploidy_calls" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CNV_metrics" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -57,10 +57,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,632 +501,632 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>HCM</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>GM16736</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>HG002</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>deletion</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="G2" s="2" t="n">
         <v>137174039</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2" s="2" t="n">
         <v>137279172</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2" s="2" t="n">
         <v>96480</v>
       </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="inlineStr">
+      <c r="J2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>HCM</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>GM16736</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>HG002</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t>deletion</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" s="2" t="n">
         <v>21814479</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3" s="2" t="n">
         <v>21837075</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3" s="2" t="n">
         <v>8595</v>
       </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="inlineStr">
+      <c r="J3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>HCM</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>GM16736</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>HG002</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
         <is>
           <t>deletion</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="2" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="G4" s="2" t="n">
         <v>18905435</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4" s="2" t="n">
         <v>18944825</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4" s="2" t="n">
         <v>37054</v>
       </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="inlineStr">
+      <c r="J4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>HCM</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>GM16736</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>HG002</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="2" t="inlineStr">
         <is>
           <t>duplication_split</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="2" t="inlineStr">
         <is>
           <t>14</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="2" t="inlineStr">
         <is>
           <t>14</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="G5" s="2" t="n">
         <v>57465816</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5" s="2" t="n">
         <v>57672657</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5" s="2" t="n">
         <v>206841</v>
       </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="inlineStr">
+      <c r="J5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>HCM</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>GM16736</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t>HG002</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
         <is>
           <t>insertion</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" s="2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="G6" t="n">
+      <c r="G6" s="2" t="n">
         <v>32697887</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6" s="2" t="n">
         <v>32727006</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6" s="2" t="n">
         <v>21603</v>
       </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="inlineStr">
+      <c r="J6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>HCM</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>GM16736</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>HG002</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="2" t="inlineStr">
         <is>
           <t>insertion</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="2" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="G7" s="2" t="n">
         <v>117928990</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7" s="2" t="n">
         <v>117940785</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7" s="2" t="n">
         <v>5762</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J7" s="2" t="n">
         <v>90</v>
       </c>
-      <c r="K7" t="n">
+      <c r="K7" s="2" t="n">
         <v>90</v>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="L7" s="2" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>HCM</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>GM16736</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>HG002</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <t>insertion</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" s="2" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="G8" t="n">
+      <c r="G8" s="2" t="n">
         <v>84587488</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8" s="2" t="n">
         <v>84636140</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8" s="2" t="n">
         <v>114960</v>
       </c>
-      <c r="J8" t="n">
+      <c r="J8" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="K8" t="n">
+      <c r="K8" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="L8" s="2" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>HCM</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>GM16736</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="2" t="inlineStr">
         <is>
           <t>HG002</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="2" t="inlineStr">
         <is>
           <t>insertion</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" s="2" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" s="2" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="G9" t="n">
+      <c r="G9" s="2" t="n">
         <v>29947958</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9" s="2" t="n">
         <v>29950614</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9" s="2" t="n">
         <v>5894</v>
       </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="inlineStr">
+      <c r="J9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>HCM</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>GM16736</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>HG002</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="2" t="inlineStr">
         <is>
           <t>translocation_interchr</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" s="2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" s="2" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="G10" t="n">
+      <c r="G10" s="2" t="n">
         <v>56528076</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H10" s="2" t="n">
         <v>62166879</v>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I10" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="inlineStr">
+      <c r="J10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>HCM</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>GM16736</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="2" t="inlineStr">
         <is>
           <t>HG002</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="2" t="inlineStr">
         <is>
           <t>translocation_interchr</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" s="2" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" s="2" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="G11" t="n">
+      <c r="G11" s="2" t="n">
         <v>64820262</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11" s="2" t="n">
         <v>57454464</v>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="I11" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="J11" t="n">
+      <c r="J11" s="2" t="n">
         <v>171</v>
       </c>
-      <c r="K11" t="n">
+      <c r="K11" s="2" t="n">
         <v>171</v>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="L11" s="2" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>HCM</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>GM16736</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>HG002</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="2" t="inlineStr">
         <is>
           <t>translocation_interchr</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E12" s="2" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" s="2" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="G12" t="n">
+      <c r="G12" s="2" t="n">
         <v>143712074</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H12" s="2" t="n">
         <v>10032710</v>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="I12" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="J12" t="n">
+      <c r="J12" s="2" t="n">
         <v>90</v>
       </c>
-      <c r="K12" t="n">
+      <c r="K12" s="2" t="n">
         <v>90</v>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="L12" s="2" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>HCM</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>GM16736</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="2" t="inlineStr">
         <is>
           <t>HG002</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="2" t="inlineStr">
         <is>
           <t>translocation_interchr</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E13" s="2" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" s="2" t="inlineStr">
         <is>
           <t>22</t>
         </is>
       </c>
-      <c r="G13" t="n">
+      <c r="G13" s="2" t="n">
         <v>21976950</v>
       </c>
-      <c r="H13" t="n">
+      <c r="H13" s="2" t="n">
         <v>20318054</v>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="I13" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="inlineStr">
+      <c r="J13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2" t="inlineStr">
         <is>
           <t>no</t>
         </is>
@@ -1259,21 +1262,21 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Percent above expected (2 Mbp window)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+          <t>Percent difference (2 Mbp window)</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>4.728</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="2" t="n">
         <v>4.728</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -1282,21 +1285,21 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Percent above expected (6 Mbp window)</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+          <t>Percent difference (2 Mbp window)</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>12.245</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="2" t="n">
         <v>12.245</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -1308,18 +1311,18 @@
           <t>Correlation with label density</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="2" t="n">
         <v>0.07000000000000001</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="2" t="n">
         <v>0.07000000000000001</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
@@ -1331,18 +1334,18 @@
           <t>Wave template correlation</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="B5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="inlineStr">
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>

</xml_diff>

<commit_message>
adding updated example output files
</commit_message>
<xml_diff>
--- a/examples/GM16736_vs_HG002/GM16736_vs_HG002.xlsx
+++ b/examples/GM16736_vs_HG002/GM16736_vs_HG002.xlsx
@@ -1262,7 +1262,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Percent difference (2 Mbp window)</t>
+          <t>Percent difference between observed and expected coefficient of variation (2 Mbp window)</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
@@ -1285,7 +1285,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Percent difference (2 Mbp window)</t>
+          <t>Percent difference between observed and expected coefficient of variation (6 Mbp window)</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">

</xml_diff>

<commit_message>
updating example output files to reflect new naming convention
</commit_message>
<xml_diff>
--- a/examples/GM16736_vs_HG002/GM16736_vs_HG002.xlsx
+++ b/examples/GM16736_vs_HG002/GM16736_vs_HG002.xlsx
@@ -446,7 +446,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Case Sample Name</t>
+          <t>Treated Sample Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -461,32 +461,32 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Case Start Chromosome</t>
+          <t>Start Chromosome</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Case End Chromosome</t>
+          <t>End Chromosome</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Case Event Start</t>
+          <t>Event Start</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Case Event End</t>
+          <t>Event End</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Case Event Size</t>
+          <t>Event Size</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Case Molecule Count</t>
+          <t>Treated Molecule Count</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -541,7 +541,7 @@
         <v>96480</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="K2" s="2" t="n">
         <v>0</v>
@@ -590,10 +590,10 @@
         <v>21837075</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>8595</v>
+        <v>8600</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="K3" s="2" t="n">
         <v>0</v>
@@ -645,7 +645,7 @@
         <v>37054</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K4" s="2" t="n">
         <v>0</v>
@@ -697,7 +697,7 @@
         <v>206841</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="K5" s="2" t="n">
         <v>0</v>
@@ -749,7 +749,7 @@
         <v>21603</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="K6" s="2" t="n">
         <v>0</v>
@@ -801,7 +801,7 @@
         <v>5762</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>90</v>
+        <v>203</v>
       </c>
       <c r="K7" s="2" t="n">
         <v>90</v>
@@ -853,7 +853,7 @@
         <v>114960</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="K8" s="2" t="n">
         <v>20</v>
@@ -905,7 +905,7 @@
         <v>5894</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="K9" s="2" t="n">
         <v>0</v>
@@ -951,7 +951,7 @@
         <v>56528076</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>62166879</v>
+        <v>62168640</v>
       </c>
       <c r="I10" s="2" t="inlineStr">
         <is>
@@ -959,7 +959,7 @@
         </is>
       </c>
       <c r="J10" s="2" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="K10" s="2" t="n">
         <v>0</v>
@@ -1013,7 +1013,7 @@
         </is>
       </c>
       <c r="J11" s="2" t="n">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>171</v>
@@ -1067,7 +1067,7 @@
         </is>
       </c>
       <c r="J12" s="2" t="n">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="K12" s="2" t="n">
         <v>90</v>
@@ -1110,10 +1110,10 @@
         </is>
       </c>
       <c r="G13" s="2" t="n">
-        <v>21976950</v>
+        <v>21982907</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>20318054</v>
+        <v>20364964</v>
       </c>
       <c r="I13" s="2" t="inlineStr">
         <is>
@@ -1121,7 +1121,7 @@
         </is>
       </c>
       <c r="J13" s="2" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="K13" s="2" t="n">
         <v>0</v>
@@ -1159,7 +1159,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Case Sample Name</t>
+          <t>Treated Sample Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -1179,27 +1179,27 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Case Chromosome</t>
+          <t>Chromosome</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Case Event Start</t>
+          <t>Event Start</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Case Event End</t>
+          <t>Event End</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Case Event Size</t>
+          <t>Event Size</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Case Fractional Copy Number</t>
+          <t>Treated Fractional Copy Number</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -1245,7 +1245,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Case QC Passed</t>
+          <t>Treated QC Passed</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
@@ -1278,7 +1278,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D3" s="2" t="n">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -1316,7 +1316,7 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D4" s="2" t="n">
@@ -1324,7 +1324,7 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="D5" s="2" t="n">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>yes</t>
         </is>
       </c>
     </row>

</xml_diff>